<commit_message>
Alteração no plano de projeto e cronogramae criacao do arquivo da nova ralease
</commit_message>
<xml_diff>
--- a/documentos/Estimativa de Tamanho do Projeto.xlsx
+++ b/documentos/Estimativa de Tamanho do Projeto.xlsx
@@ -1454,7 +1454,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="13" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="138">
+  <cellXfs count="139">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1743,50 +1743,8 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1799,6 +1757,50 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1810,19 +1812,19 @@
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1831,8 +1833,9 @@
     <xf numFmtId="0" fontId="11" fillId="6" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="6" fillId="2" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2556,7 +2559,7 @@
   <dimension ref="A1:AMK37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A6" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2604,32 +2607,32 @@
     </row>
     <row r="3" spans="1:13" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2"/>
-      <c r="B3" s="108" t="s">
+      <c r="B3" s="124" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="108"/>
-      <c r="D3" s="108"/>
-      <c r="E3" s="108"/>
-      <c r="F3" s="108"/>
-      <c r="G3" s="108"/>
-      <c r="H3" s="108"/>
-      <c r="I3" s="108"/>
-      <c r="J3" s="108"/>
+      <c r="C3" s="124"/>
+      <c r="D3" s="124"/>
+      <c r="E3" s="124"/>
+      <c r="F3" s="124"/>
+      <c r="G3" s="124"/>
+      <c r="H3" s="124"/>
+      <c r="I3" s="124"/>
+      <c r="J3" s="124"/>
       <c r="K3" s="2"/>
       <c r="L3"/>
       <c r="M3"/>
     </row>
     <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A4" s="2"/>
-      <c r="B4" s="108"/>
-      <c r="C4" s="108"/>
-      <c r="D4" s="108"/>
-      <c r="E4" s="108"/>
-      <c r="F4" s="108"/>
-      <c r="G4" s="108"/>
-      <c r="H4" s="108"/>
-      <c r="I4" s="108"/>
-      <c r="J4" s="108"/>
+      <c r="B4" s="124"/>
+      <c r="C4" s="124"/>
+      <c r="D4" s="124"/>
+      <c r="E4" s="124"/>
+      <c r="F4" s="124"/>
+      <c r="G4" s="124"/>
+      <c r="H4" s="124"/>
+      <c r="I4" s="124"/>
+      <c r="J4" s="124"/>
       <c r="K4" s="2"/>
       <c r="L4"/>
       <c r="M4"/>
@@ -2649,79 +2652,79 @@
       <c r="M5"/>
     </row>
     <row r="6" spans="1:13" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B6" s="109" t="s">
+      <c r="B6" s="125" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="109"/>
-      <c r="D6" s="110" t="s">
+      <c r="C6" s="125"/>
+      <c r="D6" s="126" t="s">
         <v>2</v>
       </c>
-      <c r="E6" s="110"/>
-      <c r="F6" s="110"/>
-      <c r="G6" s="110"/>
-      <c r="H6" s="110"/>
-      <c r="I6" s="110"/>
+      <c r="E6" s="126"/>
+      <c r="F6" s="126"/>
+      <c r="G6" s="126"/>
+      <c r="H6" s="126"/>
+      <c r="I6" s="126"/>
       <c r="J6"/>
       <c r="K6"/>
       <c r="L6"/>
       <c r="M6"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B7" s="111" t="s">
+      <c r="B7" s="120" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="111"/>
-      <c r="D7" s="112" t="s">
+      <c r="C7" s="120"/>
+      <c r="D7" s="127" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="112"/>
-      <c r="F7" s="112"/>
-      <c r="G7" s="112"/>
-      <c r="H7" s="112"/>
-      <c r="I7" s="112"/>
+      <c r="E7" s="127"/>
+      <c r="F7" s="127"/>
+      <c r="G7" s="127"/>
+      <c r="H7" s="127"/>
+      <c r="I7" s="127"/>
       <c r="J7"/>
       <c r="K7"/>
       <c r="L7"/>
       <c r="M7"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B8" s="113" t="s">
+      <c r="B8" s="119" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="113"/>
+      <c r="C8" s="119"/>
       <c r="D8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="E8" s="4"/>
-      <c r="F8" s="111" t="s">
+      <c r="F8" s="120" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="111"/>
+      <c r="G8" s="120"/>
       <c r="H8" s="3" t="s">
         <v>8</v>
       </c>
       <c r="I8" s="4"/>
       <c r="J8"/>
       <c r="K8"/>
-      <c r="L8" s="136"/>
+      <c r="L8" s="108"/>
       <c r="M8"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B9"/>
       <c r="C9" s="5"/>
-      <c r="D9" s="114" t="s">
+      <c r="D9" s="121" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="114"/>
-      <c r="F9" s="114"/>
-      <c r="G9" s="114"/>
-      <c r="H9" s="114"/>
-      <c r="I9" s="114"/>
+      <c r="E9" s="121"/>
+      <c r="F9" s="121"/>
+      <c r="G9" s="121"/>
+      <c r="H9" s="121"/>
+      <c r="I9" s="121"/>
       <c r="J9" s="6"/>
       <c r="K9"/>
-      <c r="L9" s="137">
+      <c r="L9" s="109">
         <f>J15+J16</f>
-        <v>103.46666666666667</v>
+        <v>25.866666666666667</v>
       </c>
       <c r="M9"/>
     </row>
@@ -2754,18 +2757,18 @@
       <c r="M11"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B12" s="115" t="s">
+      <c r="B12" s="122" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="115"/>
-      <c r="D12" s="115"/>
-      <c r="E12" s="115"/>
+      <c r="C12" s="122"/>
+      <c r="D12" s="122"/>
+      <c r="E12" s="122"/>
       <c r="F12"/>
-      <c r="G12" s="116" t="s">
+      <c r="G12" s="123" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="116"/>
-      <c r="I12" s="116"/>
+      <c r="H12" s="123"/>
+      <c r="I12" s="123"/>
       <c r="J12" s="7" t="s">
         <v>12</v>
       </c>
@@ -2776,24 +2779,24 @@
       <c r="M12" s="8"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B13" s="117" t="s">
+      <c r="B13" s="116" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="117"/>
-      <c r="D13" s="117"/>
+      <c r="C13" s="116"/>
+      <c r="D13" s="116"/>
       <c r="E13" s="9">
         <f>Atores!D10+'RFS ou RFC'!D10</f>
         <v>120</v>
       </c>
       <c r="F13"/>
-      <c r="G13" s="117" t="s">
+      <c r="G13" s="116" t="s">
         <v>15</v>
       </c>
-      <c r="H13" s="117"/>
-      <c r="I13" s="117"/>
+      <c r="H13" s="116"/>
+      <c r="I13" s="116"/>
       <c r="J13" s="10">
         <f t="shared" ref="J13:J20" si="0">$E$13*$E$14*K13</f>
-        <v>44.800000000000004</v>
+        <v>11.200000000000001</v>
       </c>
       <c r="K13" s="11">
         <f>dadoshistoricos!E31</f>
@@ -2803,24 +2806,23 @@
       <c r="M13" s="12"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B14" s="118" t="s">
+      <c r="B14" s="117" t="s">
         <v>16</v>
       </c>
-      <c r="C14" s="118"/>
-      <c r="D14" s="118"/>
+      <c r="C14" s="117"/>
+      <c r="D14" s="117"/>
       <c r="E14" s="13">
-        <f>dadoshistoricos!L30</f>
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="F14"/>
-      <c r="G14" s="119" t="s">
+      <c r="G14" s="115" t="s">
         <v>17</v>
       </c>
-      <c r="H14" s="119"/>
-      <c r="I14" s="119"/>
+      <c r="H14" s="115"/>
+      <c r="I14" s="115"/>
       <c r="J14" s="14">
         <f t="shared" si="0"/>
-        <v>157.86666666666667</v>
+        <v>39.466666666666669</v>
       </c>
       <c r="K14" s="15">
         <f>dadoshistoricos!F31*0.8</f>
@@ -2830,19 +2832,19 @@
       <c r="M14" s="12"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B15" s="120"/>
-      <c r="C15" s="120"/>
-      <c r="D15" s="120"/>
+      <c r="B15" s="118"/>
+      <c r="C15" s="118"/>
+      <c r="D15" s="118"/>
       <c r="E15"/>
       <c r="F15"/>
-      <c r="G15" s="119" t="s">
+      <c r="G15" s="115" t="s">
         <v>18</v>
       </c>
-      <c r="H15" s="119"/>
-      <c r="I15" s="119"/>
+      <c r="H15" s="115"/>
+      <c r="I15" s="115"/>
       <c r="J15" s="14">
         <f t="shared" si="0"/>
-        <v>39.466666666666669</v>
+        <v>9.8666666666666671</v>
       </c>
       <c r="K15" s="16">
         <f>dadoshistoricos!F31*0.2</f>
@@ -2852,19 +2854,19 @@
       <c r="M15" s="12"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B16" s="121"/>
-      <c r="C16" s="121"/>
-      <c r="D16" s="121"/>
+      <c r="B16" s="114"/>
+      <c r="C16" s="114"/>
+      <c r="D16" s="114"/>
       <c r="E16"/>
       <c r="F16"/>
-      <c r="G16" s="119" t="s">
+      <c r="G16" s="115" t="s">
         <v>19</v>
       </c>
-      <c r="H16" s="119"/>
-      <c r="I16" s="119"/>
+      <c r="H16" s="115"/>
+      <c r="I16" s="115"/>
       <c r="J16" s="14">
         <f t="shared" si="0"/>
-        <v>64</v>
+        <v>16</v>
       </c>
       <c r="K16" s="16">
         <f>dadoshistoricos!G31</f>
@@ -2879,14 +2881,14 @@
       <c r="D17"/>
       <c r="E17"/>
       <c r="F17"/>
-      <c r="G17" s="122" t="s">
+      <c r="G17" s="110" t="s">
         <v>20</v>
       </c>
-      <c r="H17" s="122"/>
-      <c r="I17" s="122"/>
-      <c r="J17" s="14">
+      <c r="H17" s="110"/>
+      <c r="I17" s="110"/>
+      <c r="J17" s="138">
         <f t="shared" si="0"/>
-        <v>533.33333333333337</v>
+        <v>133.33333333333334</v>
       </c>
       <c r="K17" s="16">
         <f>dadoshistoricos!H31</f>
@@ -2901,14 +2903,14 @@
       <c r="D18"/>
       <c r="E18"/>
       <c r="F18"/>
-      <c r="G18" s="122" t="s">
+      <c r="G18" s="110" t="s">
         <v>21</v>
       </c>
-      <c r="H18" s="122"/>
-      <c r="I18" s="122"/>
+      <c r="H18" s="110"/>
+      <c r="I18" s="110"/>
       <c r="J18" s="14">
         <f t="shared" si="0"/>
-        <v>21.333333333333336</v>
+        <v>5.3333333333333339</v>
       </c>
       <c r="K18" s="16">
         <f>dadoshistoricos!I31</f>
@@ -2922,14 +2924,14 @@
       <c r="D19"/>
       <c r="E19" s="12"/>
       <c r="F19" s="12"/>
-      <c r="G19" s="122" t="s">
+      <c r="G19" s="110" t="s">
         <v>22</v>
       </c>
-      <c r="H19" s="122"/>
-      <c r="I19" s="122"/>
+      <c r="H19" s="110"/>
+      <c r="I19" s="110"/>
       <c r="J19" s="14">
         <f t="shared" si="0"/>
-        <v>65.066666666666677</v>
+        <v>16.266666666666669</v>
       </c>
       <c r="K19" s="16">
         <f>dadoshistoricos!J31</f>
@@ -2945,14 +2947,14 @@
       <c r="D20" s="17"/>
       <c r="E20" s="17"/>
       <c r="F20" s="17"/>
-      <c r="G20" s="122" t="s">
+      <c r="G20" s="110" t="s">
         <v>24</v>
       </c>
-      <c r="H20" s="122"/>
-      <c r="I20" s="122"/>
+      <c r="H20" s="110"/>
+      <c r="I20" s="110"/>
       <c r="J20" s="14">
         <f t="shared" si="0"/>
-        <v>34.133333333333333</v>
+        <v>8.5333333333333332</v>
       </c>
       <c r="K20" s="16">
         <f>dadoshistoricos!K31</f>
@@ -2966,14 +2968,14 @@
       <c r="D21"/>
       <c r="E21"/>
       <c r="F21"/>
-      <c r="G21" s="123" t="s">
+      <c r="G21" s="111" t="s">
         <v>25</v>
       </c>
-      <c r="H21" s="123"/>
-      <c r="I21" s="123"/>
+      <c r="H21" s="111"/>
+      <c r="I21" s="111"/>
       <c r="J21" s="18">
         <f>SUM(J13:J20)</f>
-        <v>960.00000000000011</v>
+        <v>240.00000000000003</v>
       </c>
       <c r="K21" s="19">
         <f>SUM(K13:K20)</f>
@@ -2982,31 +2984,31 @@
       <c r="L21" s="12"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B22" s="124" t="s">
+      <c r="B22" s="112" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="124"/>
-      <c r="D22" s="124"/>
-      <c r="E22" s="124"/>
-      <c r="F22" s="124"/>
-      <c r="G22" s="124"/>
-      <c r="H22" s="124"/>
-      <c r="I22" s="124"/>
-      <c r="J22" s="124"/>
+      <c r="C22" s="112"/>
+      <c r="D22" s="112"/>
+      <c r="E22" s="112"/>
+      <c r="F22" s="112"/>
+      <c r="G22" s="112"/>
+      <c r="H22" s="112"/>
+      <c r="I22" s="112"/>
+      <c r="J22" s="112"/>
       <c r="L22" s="12"/>
     </row>
     <row r="23" spans="2:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B23" s="125" t="s">
+      <c r="B23" s="113" t="s">
         <v>27</v>
       </c>
-      <c r="C23" s="125"/>
-      <c r="D23" s="125"/>
-      <c r="E23" s="125"/>
-      <c r="F23" s="125"/>
-      <c r="G23" s="125"/>
-      <c r="H23" s="125"/>
-      <c r="I23" s="125"/>
-      <c r="J23" s="125"/>
+      <c r="C23" s="113"/>
+      <c r="D23" s="113"/>
+      <c r="E23" s="113"/>
+      <c r="F23" s="113"/>
+      <c r="G23" s="113"/>
+      <c r="H23" s="113"/>
+      <c r="I23" s="113"/>
+      <c r="J23" s="113"/>
       <c r="L23" s="12"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.2">
@@ -3064,50 +3066,50 @@
       <c r="L27" s="12"/>
     </row>
     <row r="28" spans="2:13" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B28" s="125" t="s">
+      <c r="B28" s="113" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="125"/>
-      <c r="D28" s="125"/>
-      <c r="E28" s="125"/>
-      <c r="F28" s="125"/>
-      <c r="G28" s="125"/>
-      <c r="H28" s="125"/>
-      <c r="I28" s="125"/>
-      <c r="J28" s="125"/>
+      <c r="C28" s="113"/>
+      <c r="D28" s="113"/>
+      <c r="E28" s="113"/>
+      <c r="F28" s="113"/>
+      <c r="G28" s="113"/>
+      <c r="H28" s="113"/>
+      <c r="I28" s="113"/>
+      <c r="J28" s="113"/>
     </row>
     <row r="37" ht="23.25" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="G21:I21"/>
-    <mergeCell ref="B22:J22"/>
-    <mergeCell ref="B23:J23"/>
-    <mergeCell ref="B28:J28"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="G16:I16"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="B3:J4"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:I6"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="D7:I7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="F8:G8"/>
+    <mergeCell ref="D9:I9"/>
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="G12:I12"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="G13:I13"/>
     <mergeCell ref="B14:D14"/>
     <mergeCell ref="G14:I14"/>
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="G15:I15"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="F8:G8"/>
-    <mergeCell ref="D9:I9"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="G12:I12"/>
-    <mergeCell ref="B3:J4"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:I6"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="D7:I7"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="G16:I16"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="B22:J22"/>
+    <mergeCell ref="B23:J23"/>
+    <mergeCell ref="B28:J28"/>
   </mergeCells>
   <pageMargins left="0.39374999999999999" right="0.39374999999999999" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
-  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3150,11 +3152,11 @@
     </row>
     <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="126" t="s">
+      <c r="B2" s="128" t="s">
         <v>32</v>
       </c>
-      <c r="C2" s="126"/>
-      <c r="D2" s="126"/>
+      <c r="C2" s="128"/>
+      <c r="D2" s="128"/>
       <c r="E2" s="21"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
@@ -3446,11 +3448,11 @@
     </row>
     <row r="2" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2"/>
-      <c r="B2" s="127" t="s">
+      <c r="B2" s="129" t="s">
         <v>43</v>
       </c>
-      <c r="C2" s="127"/>
-      <c r="D2" s="127"/>
+      <c r="C2" s="129"/>
+      <c r="D2" s="129"/>
       <c r="E2" s="44"/>
       <c r="F2" s="44"/>
       <c r="G2" s="44"/>
@@ -3562,9 +3564,9 @@
       <c r="O10"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="128"/>
-      <c r="B11" s="128"/>
-      <c r="C11" s="128"/>
+      <c r="A11" s="130"/>
+      <c r="B11" s="130"/>
+      <c r="C11" s="130"/>
       <c r="D11"/>
       <c r="E11"/>
       <c r="H11"/>
@@ -9083,12 +9085,12 @@
       <c r="M3"/>
     </row>
     <row r="4" spans="2:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="126" t="s">
+      <c r="B4" s="128" t="s">
         <v>51</v>
       </c>
-      <c r="C4" s="126"/>
-      <c r="D4" s="126"/>
-      <c r="E4" s="126"/>
+      <c r="C4" s="128"/>
+      <c r="D4" s="128"/>
+      <c r="E4" s="128"/>
       <c r="F4"/>
       <c r="G4"/>
       <c r="H4"/>
@@ -9127,12 +9129,12 @@
       <c r="M6"/>
     </row>
     <row r="7" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B7" s="129" t="s">
+      <c r="B7" s="133" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="129"/>
-      <c r="D7" s="129"/>
-      <c r="E7" s="129"/>
+      <c r="C7" s="133"/>
+      <c r="D7" s="133"/>
+      <c r="E7" s="133"/>
       <c r="F7"/>
       <c r="G7"/>
       <c r="H7" s="12"/>
@@ -9451,11 +9453,11 @@
       <c r="M21" s="12"/>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B22" s="130" t="s">
+      <c r="B22" s="132" t="s">
         <v>81</v>
       </c>
-      <c r="C22" s="130"/>
-      <c r="D22" s="130"/>
+      <c r="C22" s="132"/>
+      <c r="D22" s="132"/>
       <c r="E22" s="73">
         <f>0.6+(0.01*SUM(D9*E9,D10*E10,D11*E11,D12*E12,D13*E13,D14*E14,D15*E15,D16*E16,D17*E17,D18*E18,D19*E19,D20*E20,D21*E21))</f>
         <v>1.04</v>
@@ -9502,12 +9504,12 @@
       <c r="I25"/>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="B26" s="131" t="s">
+      <c r="B26" s="134" t="s">
         <v>82</v>
       </c>
-      <c r="C26" s="131"/>
-      <c r="D26" s="131"/>
-      <c r="E26" s="131"/>
+      <c r="C26" s="134"/>
+      <c r="D26" s="134"/>
+      <c r="E26" s="134"/>
       <c r="F26" s="74"/>
       <c r="G26" s="75"/>
       <c r="I26"/>
@@ -9516,11 +9518,11 @@
       <c r="B27" s="76" t="s">
         <v>47</v>
       </c>
-      <c r="C27" s="132" t="s">
+      <c r="C27" s="135" t="s">
         <v>53</v>
       </c>
-      <c r="D27" s="132"/>
-      <c r="E27" s="132"/>
+      <c r="D27" s="135"/>
+      <c r="E27" s="135"/>
       <c r="F27" s="76" t="s">
         <v>34</v>
       </c>
@@ -9533,11 +9535,11 @@
       <c r="B28" s="29" t="s">
         <v>83</v>
       </c>
-      <c r="C28" s="133" t="s">
+      <c r="C28" s="131" t="s">
         <v>84</v>
       </c>
-      <c r="D28" s="133"/>
-      <c r="E28" s="133"/>
+      <c r="D28" s="131"/>
+      <c r="E28" s="131"/>
       <c r="F28" s="29">
         <v>1.5</v>
       </c>
@@ -9550,11 +9552,11 @@
       <c r="B29" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="C29" s="133" t="s">
+      <c r="C29" s="131" t="s">
         <v>86</v>
       </c>
-      <c r="D29" s="133"/>
-      <c r="E29" s="133"/>
+      <c r="D29" s="131"/>
+      <c r="E29" s="131"/>
       <c r="F29" s="29">
         <v>0.5</v>
       </c>
@@ -9567,11 +9569,11 @@
       <c r="B30" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="C30" s="133" t="s">
+      <c r="C30" s="131" t="s">
         <v>88</v>
       </c>
-      <c r="D30" s="133"/>
-      <c r="E30" s="133"/>
+      <c r="D30" s="131"/>
+      <c r="E30" s="131"/>
       <c r="F30" s="29">
         <v>1</v>
       </c>
@@ -9584,11 +9586,11 @@
       <c r="B31" s="29" t="s">
         <v>89</v>
       </c>
-      <c r="C31" s="133" t="s">
+      <c r="C31" s="131" t="s">
         <v>90</v>
       </c>
-      <c r="D31" s="133"/>
-      <c r="E31" s="133"/>
+      <c r="D31" s="131"/>
+      <c r="E31" s="131"/>
       <c r="F31" s="29">
         <v>0.5</v>
       </c>
@@ -9601,11 +9603,11 @@
       <c r="B32" s="29" t="s">
         <v>91</v>
       </c>
-      <c r="C32" s="133" t="s">
+      <c r="C32" s="131" t="s">
         <v>92</v>
       </c>
-      <c r="D32" s="133"/>
-      <c r="E32" s="133"/>
+      <c r="D32" s="131"/>
+      <c r="E32" s="131"/>
       <c r="F32" s="29">
         <v>1</v>
       </c>
@@ -9618,11 +9620,11 @@
       <c r="B33" s="29" t="s">
         <v>93</v>
       </c>
-      <c r="C33" s="133" t="s">
+      <c r="C33" s="131" t="s">
         <v>94</v>
       </c>
-      <c r="D33" s="133"/>
-      <c r="E33" s="133"/>
+      <c r="D33" s="131"/>
+      <c r="E33" s="131"/>
       <c r="F33" s="29">
         <v>2</v>
       </c>
@@ -9635,11 +9637,11 @@
       <c r="B34" s="29" t="s">
         <v>95</v>
       </c>
-      <c r="C34" s="133" t="s">
+      <c r="C34" s="131" t="s">
         <v>96</v>
       </c>
-      <c r="D34" s="133"/>
-      <c r="E34" s="133"/>
+      <c r="D34" s="131"/>
+      <c r="E34" s="131"/>
       <c r="F34" s="29">
         <v>-1</v>
       </c>
@@ -9652,11 +9654,11 @@
       <c r="B35" s="29" t="s">
         <v>97</v>
       </c>
-      <c r="C35" s="133" t="s">
+      <c r="C35" s="131" t="s">
         <v>98</v>
       </c>
-      <c r="D35" s="133"/>
-      <c r="E35" s="133"/>
+      <c r="D35" s="131"/>
+      <c r="E35" s="131"/>
       <c r="F35" s="29">
         <v>-1</v>
       </c>
@@ -9666,13 +9668,13 @@
       <c r="I35" s="72"/>
     </row>
     <row r="36" spans="2:9" x14ac:dyDescent="0.2">
-      <c r="B36" s="130" t="s">
+      <c r="B36" s="132" t="s">
         <v>99</v>
       </c>
-      <c r="C36" s="130"/>
-      <c r="D36" s="130"/>
-      <c r="E36" s="130"/>
-      <c r="F36" s="130"/>
+      <c r="C36" s="132"/>
+      <c r="D36" s="132"/>
+      <c r="E36" s="132"/>
+      <c r="F36" s="132"/>
       <c r="G36" s="77">
         <f>1.4+(-0.03*SUM(F28*G28,F29*G29,F30*G30,F31*G31,F32*G32,F33*G33,F34*G34,F35*G35))</f>
         <v>1.2049999999999998</v>
@@ -9682,6 +9684,11 @@
   </sheetData>
   <sheetProtection password="C6D5" sheet="1" objects="1" scenarios="1" selectLockedCells="1"/>
   <mergeCells count="14">
+    <mergeCell ref="B4:E4"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="C27:E27"/>
     <mergeCell ref="C33:E33"/>
     <mergeCell ref="C34:E34"/>
     <mergeCell ref="C35:E35"/>
@@ -9691,11 +9698,6 @@
     <mergeCell ref="C30:E30"/>
     <mergeCell ref="C31:E31"/>
     <mergeCell ref="C32:E32"/>
-    <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B26:E26"/>
-    <mergeCell ref="C27:E27"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="whole" showErrorMessage="1" promptTitle="Influência" sqref="E9:E21 I9:I21">
@@ -9736,19 +9738,19 @@
   <sheetData>
     <row r="1" spans="1:55" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="78"/>
-      <c r="B1" s="134" t="s">
+      <c r="B1" s="136" t="s">
         <v>100</v>
       </c>
-      <c r="C1" s="134"/>
-      <c r="D1" s="134"/>
-      <c r="E1" s="134"/>
-      <c r="F1" s="134"/>
-      <c r="G1" s="134"/>
-      <c r="H1" s="134"/>
-      <c r="I1" s="134"/>
-      <c r="J1" s="134"/>
-      <c r="K1" s="134"/>
-      <c r="L1" s="134"/>
+      <c r="C1" s="136"/>
+      <c r="D1" s="136"/>
+      <c r="E1" s="136"/>
+      <c r="F1" s="136"/>
+      <c r="G1" s="136"/>
+      <c r="H1" s="136"/>
+      <c r="I1" s="136"/>
+      <c r="J1" s="136"/>
+      <c r="K1" s="136"/>
+      <c r="L1" s="136"/>
       <c r="M1" s="79"/>
       <c r="N1" s="78"/>
       <c r="O1" s="78"/>
@@ -11543,10 +11545,10 @@
       <c r="G30" s="78"/>
       <c r="H30" s="78"/>
       <c r="I30" s="78"/>
-      <c r="J30" s="135" t="s">
+      <c r="J30" s="137" t="s">
         <v>117</v>
       </c>
-      <c r="K30" s="135"/>
+      <c r="K30" s="137"/>
       <c r="L30" s="100">
         <v>8</v>
       </c>

</xml_diff>